<commit_message>
Fix vcf import issue. Auto detect existing vcf subset files.
</commit_message>
<xml_diff>
--- a/Data/Alzheimers/Posthuma_2018/AD_target_SNP.xlsx
+++ b/Data/Alzheimers/Posthuma_2018/AD_target_SNP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/Alzheimers_Data/Posthuma/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/Data/Alzheimers/Posthuma_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F804563-9D36-244B-91C0-320E33955D4A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6705AA-2290-624A-B4C9-05AB59D9FBBE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3820" yWindow="460" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case-control status (phase 1)" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="206">
   <si>
     <t>Locus</t>
   </si>
@@ -80,6 +80,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−4</t>
     </r>
@@ -94,6 +95,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -114,6 +116,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−10</t>
     </r>
@@ -137,6 +140,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−17</t>
     </r>
@@ -154,6 +158,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−10</t>
     </r>
@@ -171,6 +176,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−18</t>
     </r>
@@ -194,6 +200,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−29</t>
     </r>
@@ -208,6 +215,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−26</t>
     </r>
@@ -225,6 +233,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−44</t>
     </r>
@@ -245,6 +254,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−6</t>
     </r>
@@ -259,6 +269,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−6</t>
     </r>
@@ -276,6 +287,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−10</t>
     </r>
@@ -302,6 +314,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -331,6 +344,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -345,6 +359,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−9</t>
     </r>
@@ -371,6 +386,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -394,6 +410,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -411,6 +428,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−7</t>
     </r>
@@ -428,6 +446,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−11</t>
     </r>
@@ -448,6 +467,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−16</t>
     </r>
@@ -468,6 +488,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−9</t>
     </r>
@@ -482,6 +503,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−6</t>
     </r>
@@ -496,6 +518,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−10</t>
     </r>
@@ -516,6 +539,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−9</t>
     </r>
@@ -533,6 +557,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−10</t>
     </r>
@@ -550,6 +575,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−15</t>
     </r>
@@ -573,6 +599,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−11</t>
     </r>
@@ -590,6 +617,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−6</t>
     </r>
@@ -607,6 +635,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−11</t>
     </r>
@@ -627,6 +656,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−9</t>
     </r>
@@ -641,6 +671,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>–4</t>
     </r>
@@ -661,6 +692,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−20</t>
     </r>
@@ -678,6 +710,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−9</t>
     </r>
@@ -695,6 +728,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−19</t>
     </r>
@@ -715,6 +749,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -732,6 +767,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−5</t>
     </r>
@@ -746,6 +782,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -766,6 +803,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−13</t>
     </r>
@@ -783,6 +821,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−9</t>
     </r>
@@ -803,6 +842,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−15</t>
     </r>
@@ -823,6 +863,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−17</t>
     </r>
@@ -840,6 +881,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−11</t>
     </r>
@@ -860,6 +902,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−18</t>
     </r>
@@ -880,6 +923,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−11</t>
     </r>
@@ -894,6 +938,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−6</t>
     </r>
@@ -911,6 +956,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−11</t>
     </r>
@@ -931,6 +977,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -945,6 +992,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−6</t>
     </r>
@@ -962,6 +1010,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−10</t>
     </r>
@@ -982,6 +1031,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−4</t>
     </r>
@@ -996,6 +1046,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−7</t>
     </r>
@@ -1013,6 +1064,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−9</t>
     </r>
@@ -1033,6 +1085,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−7</t>
     </r>
@@ -1047,6 +1100,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -1067,6 +1121,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−4</t>
     </r>
@@ -1081,6 +1136,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−6</t>
     </r>
@@ -1098,6 +1154,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -1118,6 +1175,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−6</t>
     </r>
@@ -1135,6 +1193,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -1149,6 +1208,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−10</t>
     </r>
@@ -1169,6 +1229,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−5</t>
     </r>
@@ -1183,6 +1244,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−6</t>
     </r>
@@ -1197,6 +1259,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -1217,6 +1280,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−9</t>
     </r>
@@ -1234,6 +1298,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−7</t>
     </r>
@@ -1254,6 +1319,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -1280,6 +1346,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−7</t>
     </r>
@@ -1294,6 +1361,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -1314,6 +1382,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−9</t>
     </r>
@@ -1331,6 +1400,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -1348,6 +1418,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−11</t>
     </r>
@@ -1368,6 +1439,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−194</t>
     </r>
@@ -1385,6 +1457,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−296</t>
     </r>
@@ -1399,6 +1472,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−276</t>
     </r>
@@ -1419,6 +1493,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−5</t>
     </r>
@@ -1433,6 +1508,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−5</t>
     </r>
@@ -1447,6 +1523,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -1470,6 +1547,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -1484,6 +1562,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−5</t>
     </r>
@@ -1501,6 +1580,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−9</t>
     </r>
@@ -1521,6 +1601,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−8</t>
     </r>
@@ -1535,6 +1616,7 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−6</t>
     </r>
@@ -1552,9 +1634,16 @@
         <sz val="12"/>
         <color rgb="FF222222"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>−10</t>
     </r>
+  </si>
+  <si>
+    <t>CLU</t>
+  </si>
+  <si>
+    <t>PTK2B</t>
   </si>
 </sst>
 </file>
@@ -1574,6 +1663,7 @@
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1581,23 +1671,27 @@
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4240,13 +4334,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
@@ -4746,7 +4843,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>91</v>
+        <v>204</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>92</v>
@@ -4775,139 +4872,139 @@
     </row>
     <row r="16" spans="1:11" ht="18">
       <c r="A16" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E16" s="3">
-        <v>11717397</v>
+        <v>27464929</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="H16" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="I16" s="3">
-        <v>5.69</v>
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="18">
       <c r="A17" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E17" s="3">
-        <v>59958380</v>
+        <v>11717397</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="H17" s="3">
-        <v>0.38100000000000001</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>110</v>
+        <v>0.375</v>
+      </c>
+      <c r="I17" s="3">
+        <v>5.69</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="18">
       <c r="A18" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3">
         <v>11</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E18" s="3">
-        <v>85776544</v>
+        <v>59958380</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H18" s="3">
-        <v>0.314</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="18">
       <c r="A19" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="3">
         <v>11</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E19" s="3">
-        <v>121435587</v>
+        <v>85776544</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="H19" s="3">
-        <v>0.04</v>
+        <v>0.314</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>39</v>
@@ -4915,34 +5012,34 @@
     </row>
     <row r="20" spans="1:11" ht="18">
       <c r="A20" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="3">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E20" s="3">
-        <v>92938855</v>
+        <v>121435587</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="H20" s="3">
-        <v>0.34399999999999997</v>
+        <v>0.04</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>39</v>
@@ -4950,34 +5047,34 @@
     </row>
     <row r="21" spans="1:11" ht="18">
       <c r="A21" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="3">
-        <v>15</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>132</v>
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E21" s="3">
-        <v>59022615</v>
+        <v>92938855</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="H21" s="3">
-        <v>0.32</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>39</v>
@@ -4985,89 +5082,89 @@
     </row>
     <row r="22" spans="1:11" ht="18">
       <c r="A22" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="3">
         <v>15</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E22" s="3">
-        <v>63569902</v>
+        <v>59022615</v>
       </c>
       <c r="F22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="H22" s="3">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="I22" s="3">
-        <v>5.52</v>
+        <v>0.32</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="18">
       <c r="A23" s="3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E23" s="3">
-        <v>31133100</v>
+        <v>63569902</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H23" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>146</v>
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="I23" s="3">
+        <v>5.52</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="18">
       <c r="A24" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="3">
-        <v>17</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>148</v>
+        <v>16</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E24" s="3">
-        <v>5138980</v>
+        <v>31133100</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>15</v>
@@ -5076,33 +5173,33 @@
         <v>16</v>
       </c>
       <c r="H24" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="I24" s="3">
-        <v>6.12</v>
+        <v>0.3</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="18">
       <c r="A25" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="3">
         <v>17</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E25" s="3">
-        <v>47450775</v>
+        <v>5138980</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>15</v>
@@ -5111,13 +5208,13 @@
         <v>16</v>
       </c>
       <c r="H25" s="3">
-        <v>0.47299999999999998</v>
+        <v>0.12</v>
       </c>
       <c r="I25" s="3">
-        <v>5.62</v>
+        <v>6.12</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>18</v>
@@ -5131,133 +5228,133 @@
         <v>17</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E26" s="3">
-        <v>56409089</v>
+        <v>47450775</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H26" s="3">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>162</v>
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="I26" s="3">
+        <v>5.62</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="18">
       <c r="A27" s="3">
         <v>23</v>
       </c>
       <c r="B27" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E27" s="3">
-        <v>29088958</v>
+        <v>56409089</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="H27" s="3">
-        <v>0.01</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="J27" s="3">
-        <v>0.03</v>
+        <v>162</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="18">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="3">
         <v>18</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>169</v>
+      <c r="C28" s="4" t="s">
+        <v>164</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E28" s="3">
-        <v>56189459</v>
+        <v>29088958</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="H28" s="3">
-        <v>1.4E-2</v>
-      </c>
-      <c r="I28" s="3">
-        <v>5.52</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>172</v>
+        <v>0.01</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.03</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>18</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="18">
       <c r="A29" s="3">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="3">
-        <v>19</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>173</v>
+        <v>18</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E29" s="3">
-        <v>1039323</v>
+        <v>56189459</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="H29" s="3">
-        <v>0.161</v>
+        <v>1.4E-2</v>
       </c>
       <c r="I29" s="3">
-        <v>6.5</v>
+        <v>5.52</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>18</v>
@@ -5265,19 +5362,19 @@
     </row>
     <row r="30" spans="1:11" ht="18">
       <c r="A30" s="3">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="3">
         <v>19</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E30" s="3">
-        <v>45351516</v>
+        <v>1039323</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>16</v>
@@ -5286,13 +5383,13 @@
         <v>31</v>
       </c>
       <c r="H30" s="3">
-        <v>3.9E-2</v>
+        <v>0.161</v>
       </c>
       <c r="I30" s="3">
-        <v>35.5</v>
+        <v>6.5</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>18</v>
@@ -5300,106 +5397,141 @@
     </row>
     <row r="31" spans="1:11" ht="18">
       <c r="A31" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="3">
         <v>19</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>186</v>
+      <c r="C31" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E31" s="3">
-        <v>46241841</v>
+        <v>45351516</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H31" s="3">
-        <v>4.5999999999999999E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="I31" s="3">
-        <v>5.46</v>
+        <v>35.5</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>191</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="18">
       <c r="A32" s="3">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" s="3">
         <v>19</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>192</v>
+      <c r="C32" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E32" s="3">
-        <v>51727962</v>
+        <v>46241841</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H32" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>196</v>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="I32" s="3">
+        <v>5.46</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>39</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="18">
       <c r="A33" s="3">
+        <v>28</v>
+      </c>
+      <c r="B33" s="3">
+        <v>19</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E33" s="3">
+        <v>51727962</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="18">
+      <c r="A34" s="3">
         <v>29</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B34" s="3">
         <v>20</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E34" s="3">
         <v>54998544</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="3">
+      <c r="F34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="3">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I34" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="J34" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="K34" s="3" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>